<commit_message>
This commit update the talk
</commit_message>
<xml_diff>
--- a/tables/mmc2-tableS4-5.xlsx
+++ b/tables/mmc2-tableS4-5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biol. Luis Herrera\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Dropbox\r_developments\r_talks\doctoral_dissertation_FADM\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1527F713-7A1A-426C-851D-A7360358F478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="1950" yWindow="1665" windowWidth="17640" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S4" sheetId="2" r:id="rId1"/>
@@ -673,7 +674,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -785,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -810,15 +814,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -830,6 +825,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,6 +931,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -959,6 +983,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,40 +1175,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="8" width="13.5546875" customWidth="1"/>
-    <col min="9" max="10" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="10" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1199,295 +1240,295 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="15">
         <v>31.4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="15">
         <v>16.100000000000001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="15">
         <v>19</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="15">
         <v>40.4</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="15">
         <v>34.5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="15">
         <v>44.8</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="15">
         <v>37.299999999999997</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="15">
         <v>38.6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="15">
         <v>31.8</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="15">
         <v>22.8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="15">
         <v>18.899999999999999</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="15">
         <v>41.2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="15">
         <v>35.5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="15">
         <v>25.5</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="15">
         <v>33.1</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="15">
         <v>35.9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="15">
         <v>14.9</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="15">
         <v>11.4</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="15">
         <v>9.1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="15">
         <v>19.8</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="15">
         <v>15.6</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="15">
         <v>20.7</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="15">
         <v>17</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="15">
         <v>18.3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="15">
         <v>28.5</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="15">
         <v>17.3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="15">
         <v>18.100000000000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="15">
         <v>34.1</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="15">
         <v>26.9</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="15">
         <v>39.5</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="15">
         <v>19.100000000000001</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="15">
         <v>32.6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="15">
         <v>16.3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="15">
         <v>15.7</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="15">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="15">
         <v>24.3</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="15">
         <v>21.5</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="15">
         <v>20.7</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="15">
         <v>16.8</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="15">
         <v>23.2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="15">
         <v>27</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="15">
         <v>18.100000000000001</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="15">
         <v>17.899999999999999</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="15">
         <v>41.1</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="15">
         <v>63.2</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="15">
         <v>33.299999999999997</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="15">
         <v>37.9</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="15">
         <v>39.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="15">
         <v>24.4</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="15">
         <v>23.2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="15">
         <v>18.100000000000001</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="15">
         <v>32.5</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="15">
         <v>35.1</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="15">
         <v>32.4</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="15">
         <v>27.8</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="15">
         <v>30.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="15">
         <v>43</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="15">
         <v>22.8</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="15">
         <v>18.100000000000001</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="15">
         <v>47.9</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="15">
         <v>54.9</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="15">
         <v>52.2</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="15">
         <v>51.8</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="15">
         <v>50.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="15">
         <v>12.8</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="15">
         <v>10.8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="15">
         <v>11.8</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="15">
         <v>22.8</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="15">
         <v>14</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="15">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="15">
         <v>17.7</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="15">
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1528,29 +1569,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" customWidth="1"/>
-    <col min="6" max="7" width="11.77734375" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1572,237 +1613,237 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="10" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>